<commit_message>
commit view questionnaire on client page
</commit_message>
<xml_diff>
--- a/docs/táblák.xlsx
+++ b/docs/táblák.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Laravel\Eger\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEE88D3-5196-4C20-B9A2-D1D731A30794}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675CE8B4-A747-4C6E-A2E1-7EB750563983}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{69A113B1-E18D-404C-9EF8-3C552908AA5D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>clientquestionnariedetails</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>clientvoucherused</t>
   </si>
 </sst>
 </file>
@@ -458,28 +461,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F795D01-BDA7-4F35-89C4-B63FDC53A7FC}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -487,169 +493,183 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>